<commit_message>
update actions login and booking
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Get_Booking_List_Select.xlsx
+++ b/src/main/resources/input_excel_file/booking/Get_Booking_List_Select.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>tc_id</t>
   </si>
@@ -39,6 +39,12 @@
     <t>expected_result</t>
   </si>
   <si>
+    <t>partner_uid</t>
+  </si>
+  <si>
+    <t>course_uid</t>
+  </si>
+  <si>
     <t>sort_by</t>
   </si>
   <si>
@@ -64,6 +70,12 @@
   </si>
   <si>
     <t>success</t>
+  </si>
+  <si>
+    <t>CHI-LINH</t>
+  </si>
+  <si>
+    <t>CHI-LINH-01</t>
   </si>
   <si>
     <t>created_at</t>
@@ -189,18 +201,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FF1A1C1E"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF212121"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FF1A1C1E"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9.75"/>
       <color rgb="FF1A1C1E"/>
       <name val="Courier New"/>
@@ -551,7 +563,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -623,6 +635,32 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FFCCCCCC"/>
       </right>
@@ -639,12 +677,14 @@
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color rgb="FFCCCCCC"/>
       </right>
       <top style="medium">
         <color rgb="FFCCCCCC"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -771,7 +811,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -783,34 +823,34 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -895,7 +935,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -920,23 +960,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -944,14 +996,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1492,37 +1547,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="9.14285714285714" style="6"/>
     <col min="2" max="2" width="42.8571428571429" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.8571428571429" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.7142857142857" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.2857142857143" style="6" customWidth="1"/>
-    <col min="6" max="6" width="21.2857142857143" style="6" customWidth="1"/>
-    <col min="7" max="7" width="37.2857142857143" style="6" customWidth="1"/>
-    <col min="8" max="8" width="24.1428571428571" style="6" customWidth="1"/>
-    <col min="9" max="9" width="37.1428571428571" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="9.14285714285714" style="6"/>
+    <col min="3" max="5" width="21.8571428571429" style="6" customWidth="1"/>
+    <col min="6" max="6" width="23.7142857142857" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.2857142857143" style="6" customWidth="1"/>
+    <col min="8" max="8" width="21.2857142857143" style="6" customWidth="1"/>
+    <col min="9" max="9" width="37.2857142857143" style="6" customWidth="1"/>
+    <col min="10" max="10" width="24.1428571428571" style="6" customWidth="1"/>
+    <col min="11" max="11" width="37.1428571428571" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="9.14285714285714" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1" spans="1:9">
+    <row r="1" ht="27" customHeight="1" spans="1:11">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -1531,157 +1586,193 @@
       <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" ht="70" customHeight="1" spans="1:9">
-      <c r="A2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="12" t="s">
+    <row r="2" ht="70" customHeight="1" spans="1:11">
+      <c r="A2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="14" t="b">
+      <c r="E2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="15" t="b">
+      <c r="J2" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="K2" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" ht="80" customHeight="1" spans="1:11">
+      <c r="A3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" ht="80" customHeight="1" spans="1:9">
-      <c r="A3" s="16" t="s">
+    <row r="4" ht="65" customHeight="1" spans="1:11">
+      <c r="A4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="G4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="14" t="b">
+      <c r="H4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="15" t="b">
+      <c r="J4" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>19</v>
+      <c r="K4" s="24" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" ht="65" customHeight="1" spans="1:9">
-      <c r="A4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="14" t="b">
+    <row r="5" ht="78" customHeight="1" spans="1:11">
+      <c r="A5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="15" t="b">
+      <c r="J5" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>23</v>
+      <c r="K5" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:9">
-      <c r="A5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="14" t="b">
+    <row r="6" ht="63" customHeight="1" spans="1:11">
+      <c r="A6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="15" t="b">
+      <c r="J6" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" ht="63" customHeight="1" spans="1:9">
-      <c r="A6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>27</v>
+      <c r="K6" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1709,28 +1800,28 @@
   <sheetData>
     <row r="1" ht="19.5" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" ht="24" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>